<commit_message>
Final version for the thesis.
</commit_message>
<xml_diff>
--- a/Tests/Iteration_number_test-dataset1.xlsx
+++ b/Tests/Iteration_number_test-dataset1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Prace domowe\Studia IV rok\AGH\Inżynierka\Project\Tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA1B639-EB4C-4287-8279-2F69DA6909D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72C4134-5146-440A-9D6C-4973C1E88836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30780" yWindow="2835" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -430,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +443,7 @@
     <col min="5" max="7" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -466,7 +466,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>20000</v>
       </c>
@@ -488,8 +488,11 @@
       <c r="G2">
         <v>2.0382449626922599</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>10000</v>
       </c>
@@ -511,8 +514,11 @@
       <c r="G3">
         <v>0.99870896339416504</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>7500</v>
       </c>
@@ -535,7 +541,7 @@
         <v>0.736375331878662</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>5000</v>
       </c>
@@ -558,7 +564,7 @@
         <v>0.51984548568725497</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3500</v>
       </c>
@@ -581,7 +587,7 @@
         <v>0.355886220932006</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2000</v>
       </c>
@@ -604,7 +610,7 @@
         <v>0.20386552810668901</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>1000</v>
       </c>
@@ -627,7 +633,7 @@
         <v>0.100461483001708</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>500</v>
       </c>
@@ -650,18 +656,8 @@
         <v>4.8636198043823201E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>